<commit_message>
new picklefiles and other things
added picklefiles with cimbined features from physicochemical and substitution matrices. also added the code to do this and removed an old file containing my notes, the up-to-date one is still theere and renamed so it no longer ends in '(2)'
</commit_message>
<xml_diff>
--- a/data/protein_info.xlsx
+++ b/data/protein_info.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1" documentId="11_F25DC773A252ABDACC10487BF91F70425BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82603748-1459-4C37-B672-54BB577580B6}"/>
   <bookViews>
-    <workbookView xWindow="3984" yWindow="3216" windowWidth="14904" windowHeight="9168" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2304" yWindow="2304" windowWidth="14904" windowHeight="9768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -498,7 +498,7 @@
   <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>